<commit_message>
this is a automatic commit
</commit_message>
<xml_diff>
--- a/teste.xlsx
+++ b/teste.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44045C35-3EB2-4A19-93E8-8218A7B98ACB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2848CFF-1938-4F51-9955-B8AC0D7BA5FB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="960" yWindow="2380" windowWidth="19200" windowHeight="10160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -341,10 +341,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -374,6 +374,11 @@
         <v>5</v>
       </c>
     </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>